<commit_message>
added some color highlighting to the PDF hours form
</commit_message>
<xml_diff>
--- a/emt-bootcamp/PDH_Hours.xlsx
+++ b/emt-bootcamp/PDH_Hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307E581D-4FDF-4882-9263-9C2500C6FA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1C9403-EEC8-4EB1-B34A-F7A2498B7312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6430" yWindow="3830" windowWidth="18300" windowHeight="14420" xr2:uid="{56897687-6524-4104-AEE4-9C7458D0204F}"/>
+    <workbookView xWindow="6430" yWindow="3830" windowWidth="20210" windowHeight="5480" xr2:uid="{56897687-6524-4104-AEE4-9C7458D0204F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,19 +38,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>0 or 1</t>
   </si>
   <si>
-    <t>Title</t>
+    <t>Electromagnetic Transients (EMT) Boot Camp</t>
   </si>
   <si>
-    <t>Electromagnetic Transients (EMT) Boot Camp</t>
+    <t>Name to Appear on Certificate</t>
+  </si>
+  <si>
+    <t>Certificate Title</t>
+  </si>
+  <si>
+    <t>your email address</t>
   </si>
 </sst>
 </file>
@@ -74,12 +74,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -94,11 +100,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -418,22 +425,22 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
     <col min="4" max="4" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2">
         <v>45141</v>
@@ -446,14 +453,16 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>